<commit_message>
update simualtions to include Daniel's absolute data
</commit_message>
<xml_diff>
--- a/metabolite_data/fermentation data for dataset 2.xlsx
+++ b/metabolite_data/fermentation data for dataset 2.xlsx
@@ -1,20 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28209"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D05B4C8C-AF57-4813-8334-D336073912AB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/satyakam/Dropbox/Work/component_contribution_ctherm/metabolite_data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="34560" windowHeight="15468" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="34560" windowHeight="15460"/>
   </bookViews>
   <sheets>
     <sheet name="combined" sheetId="3" r:id="rId1"/>
     <sheet name="EtOH+" sheetId="1" r:id="rId2"/>
     <sheet name="control" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -81,7 +91,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -169,7 +179,7 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -239,6 +249,7 @@
     <xf numFmtId="2" fontId="2" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -263,7 +274,6 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -543,69 +553,69 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB5E1EE4-96AB-4D74-9BAF-109FA7215A8E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:P11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9:P11"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B2" s="23" t="s">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="22"/>
+      <c r="D2" s="23"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="25"/>
-      <c r="I2" s="26" t="s">
+      <c r="H2" s="26"/>
+      <c r="I2" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="26"/>
-      <c r="K2" s="27" t="s">
+      <c r="J2" s="27"/>
+      <c r="K2" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="27"/>
-      <c r="M2" s="28" t="s">
+      <c r="L2" s="28"/>
+      <c r="M2" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="28"/>
-      <c r="O2" s="21" t="s">
+      <c r="N2" s="29"/>
+      <c r="O2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="P2" s="21"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B3" s="23"/>
-      <c r="C3" s="22" t="s">
+      <c r="P2" s="22"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B3" s="24"/>
+      <c r="C3" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22" t="s">
+      <c r="D3" s="23"/>
+      <c r="E3" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="22"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="27"/>
-      <c r="L3" s="27"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
-      <c r="O3" s="21"/>
-      <c r="P3" s="21"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B4" s="24"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="22"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B4" s="25"/>
       <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
@@ -649,8 +659,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" s="29" t="s">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" s="21" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="14" t="s">
@@ -708,8 +718,8 @@
         <v>5.1207427405699999</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" s="29" t="s">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" s="21" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="14" t="s">
@@ -767,8 +777,8 @@
         <v>20.2056630091</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7" s="29" t="s">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" s="21" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="14" t="s">
@@ -826,7 +836,7 @@
         <v>40.379868086169999</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -884,7 +894,7 @@
         <v>0.20040449999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -942,7 +952,7 @@
         <v>0.47221750000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1017,69 +1027,69 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="22"/>
+      <c r="C2" s="23"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="25"/>
-      <c r="H2" s="26" t="s">
+      <c r="G2" s="26"/>
+      <c r="H2" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="26"/>
-      <c r="J2" s="27" t="s">
+      <c r="I2" s="27"/>
+      <c r="J2" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="27"/>
-      <c r="L2" s="28" t="s">
+      <c r="K2" s="28"/>
+      <c r="L2" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="28"/>
-      <c r="N2" s="21" t="s">
+      <c r="M2" s="29"/>
+      <c r="N2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="O2" s="21"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="23"/>
-      <c r="B3" s="22" t="s">
+      <c r="O2" s="22"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="24"/>
+      <c r="B3" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22" t="s">
+      <c r="C3" s="23"/>
+      <c r="D3" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="22"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="27"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="24"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="25"/>
       <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
@@ -1123,7 +1133,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>11</v>
       </c>
@@ -1179,7 +1189,7 @@
         <v>5.1207427405699999</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>12</v>
       </c>
@@ -1235,7 +1245,7 @@
         <v>20.2056630091</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>13</v>
       </c>
@@ -1308,70 +1318,70 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A32F7A9-6892-42FC-B0A8-296F7817E7CE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5:O7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15" ht="7.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
+    <row r="1" spans="1:15" ht="7.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="22"/>
+      <c r="C2" s="23"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="25"/>
-      <c r="H2" s="26" t="s">
+      <c r="G2" s="26"/>
+      <c r="H2" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="26"/>
-      <c r="J2" s="27" t="s">
+      <c r="I2" s="27"/>
+      <c r="J2" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="27"/>
-      <c r="L2" s="28" t="s">
+      <c r="K2" s="28"/>
+      <c r="L2" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="28"/>
-      <c r="N2" s="21" t="s">
+      <c r="M2" s="29"/>
+      <c r="N2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="O2" s="21"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="23"/>
-      <c r="B3" s="22" t="s">
+      <c r="O2" s="22"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="24"/>
+      <c r="B3" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22" t="s">
+      <c r="C3" s="23"/>
+      <c r="D3" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="22"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="27"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="24"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="25"/>
       <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
@@ -1415,7 +1425,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>11</v>
       </c>
@@ -1470,7 +1480,7 @@
         <v>0.20040449999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>12</v>
       </c>
@@ -1525,7 +1535,7 @@
         <v>0.47221750000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>13</v>
       </c>

</xml_diff>